<commit_message>
Alignment fixes and other small fixes
</commit_message>
<xml_diff>
--- a/data/cv_work_experience.xlsx
+++ b/data/cv_work_experience.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">formatting</t>
   </si>
   <si>
-    <t xml:space="preserve">Erhvervserfaring</t>
+    <t xml:space="preserve">Experience</t>
   </si>
   <si>
     <t xml:space="preserve">2368-72</t>
@@ -198,10 +198,10 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>

</xml_diff>